<commit_message>
fully decomposed paper and created associated example json
</commit_message>
<xml_diff>
--- a/CompleteExample/doc1/tract1.xlsx
+++ b/CompleteExample/doc1/tract1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\gitDir\WMAD\CompleteExample\doc1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370470AD-5E89-44E8-8BC2-387E35958714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13821F31-5ED7-4F29-B871-86957CFCA922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -73,12 +73,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -105,23 +99,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -341,7 +330,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -363,7 +352,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -372,7 +361,7 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -390,13 +379,6 @@
       <c r="E3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{13FA74AA-A323-429E-B34B-D81482DD8B68}"/>
-    <hyperlink ref="B2" r:id="rId2" location=":~:text=We%20begin%20by,ILF%3B%20Davis%201921)." xr:uid="{2AD7D8A8-FA36-456B-A046-BCE1DCF02C14}"/>
-    <hyperlink ref="C2" r:id="rId3" location=":~:text=The%20proportion%20of,et%20al.%202011)." xr:uid="{C1D5AC36-4BBE-4547-AA60-439BBC5F806A}"/>
-    <hyperlink ref="D2" r:id="rId4" location=":~:text=One%20of%20the,respectively%3B%20Fig.%C2%A05b)." xr:uid="{2741125C-94DF-498E-BF86-06FAC50B35FD}"/>
-    <hyperlink ref="E2" r:id="rId5" location=":~:text=In%20addition%20to%20sharing,7%2C%208%2C%20and%2014)." xr:uid="{641A0479-793F-481E-B22C-5ED48737314B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>